<commit_message>
reformating xlsx file a bit
</commit_message>
<xml_diff>
--- a/specs/admin-api-monitor-specs.xlsx
+++ b/specs/admin-api-monitor-specs.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="true"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - AdminApiMonitor Metri" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1 - AdminApiMonitor Metri" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -269,30 +274,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -305,7 +292,7 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -326,14 +313,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
@@ -349,105 +336,396 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFFFF"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:IV52"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F47" activeCellId="0" sqref="F47"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="1" width="9.0037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="37.5185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.4814814814815"/>
-    <col collapsed="false" hidden="false" max="256" min="9" style="1" width="9.0037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="9.0037037037037"/>
+    <col min="1" max="1" width="17.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" customWidth="1"/>
+    <col min="3" max="5" width="8.625" style="2"/>
+    <col min="6" max="6" width="40" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19" style="2" customWidth="1"/>
+    <col min="9" max="256" width="8.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="20.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -472,7 +750,7 @@
       </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="31" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -493,7 +771,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" ht="20.25" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -512,7 +790,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" ht="20.25" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -531,7 +809,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="20.25" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -550,7 +828,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" ht="20.25" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -569,7 +847,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" ht="20.25" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -588,7 +866,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" ht="20.25" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -607,7 +885,7 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" ht="20.25" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -626,7 +904,7 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" ht="20.25" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -645,7 +923,7 @@
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" ht="20.25" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -664,7 +942,7 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" ht="20.25" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -683,7 +961,7 @@
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" ht="20.25" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -702,7 +980,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" ht="20.25" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -721,7 +999,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" ht="20.25" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -740,7 +1018,7 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" ht="33.5" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -759,7 +1037,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" ht="20.25" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
@@ -780,7 +1058,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" ht="32.25" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -799,7 +1077,7 @@
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" ht="20.25" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
@@ -818,7 +1096,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" ht="20.25" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
@@ -837,7 +1115,7 @@
       </c>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" ht="20.25" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
@@ -856,7 +1134,7 @@
       </c>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:9" ht="20.25" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -875,7 +1153,7 @@
       </c>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" ht="20.25" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -894,7 +1172,7 @@
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" ht="20.25" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
@@ -913,7 +1191,7 @@
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:9" ht="20.25" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
@@ -932,7 +1210,7 @@
       </c>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" ht="27" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -953,7 +1231,7 @@
       </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:9" ht="20.25" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>47</v>
       </c>
@@ -972,7 +1250,7 @@
       </c>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" ht="20.25" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>49</v>
       </c>
@@ -991,7 +1269,7 @@
       </c>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" ht="20.25" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
@@ -1010,7 +1288,7 @@
       </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:9" ht="32.25" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
@@ -1029,7 +1307,7 @@
       </c>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" ht="33" customHeight="1">
       <c r="A32" s="3" t="s">
         <v>52</v>
       </c>
@@ -1050,7 +1328,7 @@
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:9" ht="33" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>53</v>
       </c>
@@ -1067,7 +1345,7 @@
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:9" ht="20.25" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>55</v>
       </c>
@@ -1086,7 +1364,7 @@
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:9" ht="20.25" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -1105,7 +1383,7 @@
       </c>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:9" ht="20.25" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>58</v>
       </c>
@@ -1124,227 +1402,227 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:9" ht="18" customHeight="1">
+      <c r="A37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="1" t="s">
+      <c r="B37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:9" ht="18" customHeight="1">
+      <c r="A38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:9" ht="18" customHeight="1">
+      <c r="A39" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="1" t="s">
+      <c r="B39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:9" ht="18" customHeight="1">
+      <c r="A40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="1" t="s">
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:9" ht="18" customHeight="1">
+      <c r="A41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="B41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:9" ht="18" customHeight="1">
+      <c r="A42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="C42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:9" ht="18" customHeight="1">
+      <c r="A43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="1" t="s">
+      <c r="D43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:9" ht="18" customHeight="1">
+      <c r="A44" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="1" t="s">
+      <c r="B44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:9" ht="18" customHeight="1">
+      <c r="A45" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="1" t="s">
+      <c r="B45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:9" ht="18" customHeight="1">
+      <c r="A46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="1" t="s">
+      <c r="C46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:9" ht="18" customHeight="1">
+      <c r="A47" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
+      <c r="B47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:9" ht="18" customHeight="1">
+      <c r="A48" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:8" ht="18" customHeight="1">
+      <c r="A49" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H49" s="1" t="s">
+      <c r="B49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:8" ht="18" customHeight="1">
+      <c r="A50" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="1" t="s">
+      <c r="B50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:8" ht="18" customHeight="1">
+      <c r="A51" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="B51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:8" ht="18" customHeight="1">
+      <c r="A52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H52" s="1" t="s">
+      <c r="B52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1352,12 +1630,15 @@
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.5"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>